<commit_message>
created new evs_SAPorder_related class
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTAMain2705.xlsx
+++ b/src/test/resources/data/jdgroupTAMain2705.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6618BE1E-3833-4CF0-B1D8-819503955C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3803026D-D5AC-4569-9D20-2A664B2EDD35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVS" sheetId="82" r:id="rId1"/>
@@ -17,64 +17,65 @@
     <sheet name="evs_PayUPagePayment++" sheetId="85" r:id="rId7"/>
     <sheet name="evs_DeliveryPopulation++" sheetId="84" r:id="rId8"/>
     <sheet name="evs_ProductSearch++" sheetId="83" r:id="rId9"/>
-    <sheet name="IC" sheetId="23" r:id="rId10"/>
-    <sheet name="evs_Login++" sheetId="81" r:id="rId11"/>
-    <sheet name="SapRSIGetDataFromSAPDB++" sheetId="80" r:id="rId12"/>
-    <sheet name="icInvalidEmailNewsLetter++" sheetId="77" r:id="rId13"/>
-    <sheet name="ic_SubscribeNewsletter++" sheetId="78" r:id="rId14"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId15"/>
-    <sheet name="IC_ClearWishList++" sheetId="66" r:id="rId16"/>
-    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId17"/>
-    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId18"/>
-    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId19"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId20"/>
-    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId21"/>
-    <sheet name="EnterContact++" sheetId="58" r:id="rId22"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId23"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId24"/>
-    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId25"/>
-    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId26"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId27"/>
-    <sheet name="giftCardReport++" sheetId="54" r:id="rId28"/>
-    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId29"/>
-    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId30"/>
-    <sheet name="SapCustomer++" sheetId="50" r:id="rId31"/>
-    <sheet name="Suites" sheetId="22" r:id="rId32"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId33"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId34"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId35"/>
-    <sheet name="RetrieveCustomerDetailsOld++" sheetId="70" r:id="rId36"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId37"/>
-    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId38"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId39"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId40"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId41"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId42"/>
-    <sheet name="IC_WishlistToCart++" sheetId="71" r:id="rId43"/>
-    <sheet name="Products_Category" sheetId="69" r:id="rId44"/>
-    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId45"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId46"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId47"/>
-    <sheet name="ClearCart++" sheetId="73" r:id="rId48"/>
-    <sheet name="ic_invalidCredslogin++" sheetId="74" r:id="rId49"/>
-    <sheet name="SendWishlistToEmail++" sheetId="75" r:id="rId50"/>
-    <sheet name="icEmailWishlistverification++" sheetId="76" r:id="rId51"/>
-    <sheet name="DB_connection_master++" sheetId="47" r:id="rId52"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId53"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId54"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId55"/>
-    <sheet name="icSearchNoResultsReturned++" sheetId="79" r:id="rId56"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId57"/>
-    <sheet name="Russels" sheetId="26" r:id="rId58"/>
-    <sheet name="Login++" sheetId="25" r:id="rId59"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId60"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId61"/>
-    <sheet name="Preferred Store" sheetId="68" r:id="rId62"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId63"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId64"/>
+    <sheet name="evs_SAP_OrderRelated++" sheetId="91" r:id="rId10"/>
+    <sheet name="IC" sheetId="23" r:id="rId11"/>
+    <sheet name="evs_Login++" sheetId="81" r:id="rId12"/>
+    <sheet name="SapRSIGetDataFromSAPDB++" sheetId="80" r:id="rId13"/>
+    <sheet name="icInvalidEmailNewsLetter++" sheetId="77" r:id="rId14"/>
+    <sheet name="ic_SubscribeNewsletter++" sheetId="78" r:id="rId15"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId16"/>
+    <sheet name="IC_ClearWishList++" sheetId="66" r:id="rId17"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId18"/>
+    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId19"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId20"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId21"/>
+    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId22"/>
+    <sheet name="EnterContact++" sheetId="58" r:id="rId23"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId24"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId25"/>
+    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId26"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId27"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId28"/>
+    <sheet name="giftCardReport++" sheetId="54" r:id="rId29"/>
+    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId30"/>
+    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId31"/>
+    <sheet name="SapCustomer++" sheetId="50" r:id="rId32"/>
+    <sheet name="Suites" sheetId="22" r:id="rId33"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId34"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId35"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId36"/>
+    <sheet name="RetrieveCustomerDetailsOld++" sheetId="70" r:id="rId37"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId38"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId39"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId40"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId41"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId42"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId43"/>
+    <sheet name="IC_WishlistToCart++" sheetId="71" r:id="rId44"/>
+    <sheet name="Products_Category" sheetId="69" r:id="rId45"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId46"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId47"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId48"/>
+    <sheet name="ClearCart++" sheetId="73" r:id="rId49"/>
+    <sheet name="ic_invalidCredslogin++" sheetId="74" r:id="rId50"/>
+    <sheet name="SendWishlistToEmail++" sheetId="75" r:id="rId51"/>
+    <sheet name="icEmailWishlistverification++" sheetId="76" r:id="rId52"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId53"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId54"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId55"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId56"/>
+    <sheet name="icSearchNoResultsReturned++" sheetId="79" r:id="rId57"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId58"/>
+    <sheet name="Russels" sheetId="26" r:id="rId59"/>
+    <sheet name="Login++" sheetId="25" r:id="rId60"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId61"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId62"/>
+    <sheet name="Preferred Store" sheetId="68" r:id="rId63"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId64"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId65"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">IC!$A$1:$S$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">IC!$A$1:$S$71</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -148,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3355" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3359" uniqueCount="811">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2586,6 +2587,9 @@
   </si>
   <si>
     <t>Ottawa Dining Chair</t>
+  </si>
+  <si>
+    <t>evs_SAP_OrderRelated</t>
   </si>
 </sst>
 </file>
@@ -5039,8 +5043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -5191,7 +5195,7 @@
         <v>801</v>
       </c>
       <c r="O3" s="175" t="s">
-        <v>193</v>
+        <v>810</v>
       </c>
       <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
@@ -5398,7 +5402,7 @@
     <hyperlink ref="N3" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{AF65DDC1-BC55-4F97-94C2-567709144F84}"/>
     <hyperlink ref="G4" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{F24D25DF-65AE-4F4B-8F4D-B77BAC52BE25}"/>
     <hyperlink ref="G5:G8" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{FED56092-5649-48DF-A585-63066B278E7F}"/>
-    <hyperlink ref="O3" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{5190E0E6-63DB-41FB-A662-5AF845A68BBC}"/>
+    <hyperlink ref="O3" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{5190E0E6-63DB-41FB-A662-5AF845A68BBC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5406,6 +5410,53 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8053730A-FA6E-4611-B67E-6C605352FBEE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="108" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>776</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z93"/>
   <sheetViews>
@@ -5413,7 +5464,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22:B26"/>
+      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -9227,7 +9278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -9287,7 +9338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -9502,7 +9553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -9552,7 +9603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -9608,7 +9659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -9713,7 +9764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -9878,7 +9929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -10103,7 +10154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -10504,98 +10555,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="38">
-        <v>49</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>510</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="38">
-        <v>50</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>511</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="38">
-        <v>51</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>512</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>388</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AA52A1-8777-405C-9238-AAC23BF8D2E8}">
   <dimension ref="A1:F14"/>
@@ -10878,6 +10837,98 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="38">
+        <v>49</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>510</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="38">
+        <v>50</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>511</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="38">
+        <v>51</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>512</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -10940,7 +10991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -11108,7 +11159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -11239,7 +11290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -11397,7 +11448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -11513,7 +11564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -11787,7 +11838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -11858,7 +11909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -11913,7 +11964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -12004,7 +12055,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B49059-B6B7-4E90-8F6A-41E8AD5AEA44}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="108" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="108" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="108" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="108" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="108" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="108"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="117" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="117" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" s="117" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="112">
+        <v>101</v>
+      </c>
+      <c r="B2" s="112" t="s">
+        <v>798</v>
+      </c>
+      <c r="C2" s="112">
+        <v>1</v>
+      </c>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -12672,62 +12778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B49059-B6B7-4E90-8F6A-41E8AD5AEA44}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" style="108" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="108" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="108" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="108" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="108" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="108"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="117" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="117" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="117" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="112">
-        <v>101</v>
-      </c>
-      <c r="B2" s="112" t="s">
-        <v>798</v>
-      </c>
-      <c r="C2" s="112">
-        <v>1</v>
-      </c>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112" t="s">
-        <v>261</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -13394,7 +13445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -13857,7 +13908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -14046,7 +14097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -14493,7 +14544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -14730,7 +14781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
@@ -15612,7 +15663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -15782,7 +15833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -15957,12 +16008,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16156,18 +16207,10 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="16">
-        <v>101</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>776</v>
-      </c>
-      <c r="C14" s="112">
-        <v>1</v>
-      </c>
-      <c r="D14" s="112" t="s">
-        <v>182</v>
-      </c>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="16"/>
@@ -16199,266 +16242,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
     <cfRule type="duplicateValues" dxfId="33" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
-  <dimension ref="A1:F13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="16">
-        <v>26</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>539</v>
-      </c>
-      <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="16">
-        <v>10</v>
-      </c>
-      <c r="E2" s="16">
-        <v>240</v>
-      </c>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="16">
-        <v>27</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>538</v>
-      </c>
-      <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16">
-        <v>10</v>
-      </c>
-      <c r="E3" s="16">
-        <v>240</v>
-      </c>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1">
-      <c r="A4" s="16">
-        <v>28</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="C4" s="16">
-        <v>1</v>
-      </c>
-      <c r="D4" s="16">
-        <v>10</v>
-      </c>
-      <c r="E4" s="16">
-        <v>240</v>
-      </c>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="16">
-        <v>29</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>536</v>
-      </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16">
-        <v>10</v>
-      </c>
-      <c r="E5" s="16">
-        <v>240</v>
-      </c>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="16">
-        <v>30</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>535</v>
-      </c>
-      <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="16">
-        <v>10</v>
-      </c>
-      <c r="E6" s="16">
-        <v>240</v>
-      </c>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="16">
-        <v>31</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>502</v>
-      </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="16">
-        <v>10</v>
-      </c>
-      <c r="E7" s="16">
-        <v>240</v>
-      </c>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="16">
-        <v>32</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>534</v>
-      </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="16">
-        <v>10</v>
-      </c>
-      <c r="E8" s="16">
-        <v>240</v>
-      </c>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="16">
-        <v>33</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>533</v>
-      </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="16">
-        <v>10</v>
-      </c>
-      <c r="E9" s="16">
-        <v>240</v>
-      </c>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="16">
-        <v>34</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>532</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16">
-        <v>10</v>
-      </c>
-      <c r="E10" s="16">
-        <v>240</v>
-      </c>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="42" t="s">
-        <v>298</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="C11" s="16">
-        <v>1</v>
-      </c>
-      <c r="D11" s="16">
-        <v>10</v>
-      </c>
-      <c r="E11" s="16">
-        <v>240</v>
-      </c>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="42" t="s">
-        <v>409</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1</v>
-      </c>
-      <c r="D12" s="16">
-        <v>10</v>
-      </c>
-      <c r="E12" s="16">
-        <v>240</v>
-      </c>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="42" t="s">
-        <v>410</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="C13" s="16">
-        <v>1</v>
-      </c>
-      <c r="D13" s="16">
-        <v>10</v>
-      </c>
-      <c r="E13" s="16">
-        <v>240</v>
-      </c>
-      <c r="F13" s="43"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16899,6 +16682,266 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="16">
+        <v>26</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>10</v>
+      </c>
+      <c r="E2" s="16">
+        <v>240</v>
+      </c>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="16">
+        <v>27</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
+        <v>10</v>
+      </c>
+      <c r="E3" s="16">
+        <v>240</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1">
+      <c r="A4" s="16">
+        <v>28</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>10</v>
+      </c>
+      <c r="E4" s="16">
+        <v>240</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="16">
+        <v>29</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16">
+        <v>240</v>
+      </c>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16">
+        <v>30</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16">
+        <v>240</v>
+      </c>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16">
+        <v>31</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>502</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>10</v>
+      </c>
+      <c r="E7" s="16">
+        <v>240</v>
+      </c>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16">
+        <v>32</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>10</v>
+      </c>
+      <c r="E8" s="16">
+        <v>240</v>
+      </c>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16">
+        <v>33</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>10</v>
+      </c>
+      <c r="E9" s="16">
+        <v>240</v>
+      </c>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16">
+        <v>34</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>10</v>
+      </c>
+      <c r="E10" s="16">
+        <v>240</v>
+      </c>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>240</v>
+      </c>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>10</v>
+      </c>
+      <c r="E12" s="16">
+        <v>240</v>
+      </c>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="42" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <v>10</v>
+      </c>
+      <c r="E13" s="16">
+        <v>240</v>
+      </c>
+      <c r="F13" s="43"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B11:B13">
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -17155,7 +17198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
@@ -17852,7 +17895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -18089,7 +18132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -18152,7 +18195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A18"/>
   <sheetViews>
@@ -18247,7 +18290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -18357,7 +18400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -18441,7 +18484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -18940,7 +18983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -19112,101 +19155,6 @@
   <conditionalFormatting sqref="B5:B7">
     <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="101" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="101" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="101" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="101" t="s">
-        <v>581</v>
-      </c>
-      <c r="E1" s="101" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="101" t="s">
-        <v>582</v>
-      </c>
-      <c r="G1" s="101" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="102">
-        <v>62</v>
-      </c>
-      <c r="B2" s="103" t="s">
-        <v>557</v>
-      </c>
-      <c r="C2" s="101">
-        <v>1</v>
-      </c>
-      <c r="D2" s="101" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="101" t="s">
-        <v>583</v>
-      </c>
-      <c r="F2" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="100" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="102">
-        <v>63</v>
-      </c>
-      <c r="B3" s="103" t="s">
-        <v>557</v>
-      </c>
-      <c r="C3" s="101">
-        <v>1</v>
-      </c>
-      <c r="D3" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="101" t="s">
-        <v>348</v>
-      </c>
-      <c r="F3" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="100" t="s">
-        <v>584</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-2900-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19260,6 +19208,101 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="101" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="101" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="101" t="s">
+        <v>581</v>
+      </c>
+      <c r="E1" s="101" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="101" t="s">
+        <v>582</v>
+      </c>
+      <c r="G1" s="101" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="102">
+        <v>62</v>
+      </c>
+      <c r="B2" s="103" t="s">
+        <v>557</v>
+      </c>
+      <c r="C2" s="101">
+        <v>1</v>
+      </c>
+      <c r="D2" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="101" t="s">
+        <v>583</v>
+      </c>
+      <c r="F2" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="100" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="102">
+        <v>63</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>557</v>
+      </c>
+      <c r="C3" s="101">
+        <v>1</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="101" t="s">
+        <v>348</v>
+      </c>
+      <c r="F3" s="101" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="100" t="s">
+        <v>584</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-2900-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -19315,7 +19358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -19423,7 +19466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -19555,7 +19598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -19692,7 +19735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -19749,7 +19792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -20237,7 +20280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -20278,7 +20321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:T32"/>
   <sheetViews>
@@ -21460,7 +21503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -21561,210 +21604,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21824,6 +21663,210 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -21927,7 +21970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -22031,7 +22074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:A71"/>
   <sheetViews>
@@ -22404,7 +22447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -22508,7 +22551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -22848,7 +22891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4572D4E6-A74B-4556-86D1-340F9ECF2463}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -24020,15 +24063,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -24037,7 +24071,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24186,24 +24220,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -24211,7 +24237,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24228,4 +24254,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>